<commit_message>
adding newest press release + updating price
</commit_message>
<xml_diff>
--- a/ATLX.xlsx
+++ b/ATLX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Library/CloudStorage/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDFFF48-60BE-064B-B3BA-1FA1E2CE7C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9E1C3-B8A3-E543-A5D8-F210B5A99B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="1440" windowWidth="35760" windowHeight="27360" xr2:uid="{67390AD3-CEA6-C848-8F5B-D66C54D1BD79}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="model" sheetId="2" r:id="rId2"/>
     <sheet name="Drill Holes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Price</t>
   </si>
@@ -55,9 +54,6 @@
     <t>Atlas Lithium Corporation</t>
   </si>
   <si>
-    <t>Q323</t>
-  </si>
-  <si>
     <t xml:space="preserve">About </t>
   </si>
   <si>
@@ -143,6 +139,12 @@
   </si>
   <si>
     <t>Depth Encountered (m)</t>
+  </si>
+  <si>
+    <t>Q1224</t>
+  </si>
+  <si>
+    <t>plant entering final stages</t>
   </si>
 </sst>
 </file>
@@ -559,7 +561,7 @@
   <dimension ref="B2:L56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -577,50 +579,50 @@
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3">
         <v>0.4511</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>15.66</v>
+        <v>15.81</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3">
         <v>0.2742</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>10.72926</v>
+        <v>14.802025</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -629,7 +631,7 @@
       </c>
       <c r="K6">
         <f>+K4*K5</f>
-        <v>168.02021160000001</v>
+        <v>234.02001525</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -637,97 +639,105 @@
         <v>3</v>
       </c>
       <c r="K7">
-        <v>22.857357</v>
+        <v>17.529464999999998</v>
       </c>
       <c r="L7" t="str">
         <f>+L5</f>
-        <v>Q323</v>
+        <v>Q1224</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="L8" t="str">
         <f>+L7</f>
-        <v>Q323</v>
+        <v>Q1224</v>
       </c>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7">
+        <v>45419</v>
+      </c>
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="E36" s="7">
         <v>45299</v>
       </c>
     </row>
@@ -741,14 +751,15 @@
         <v>43852</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B35" r:id="rId1" xr:uid="{6BBF0ACA-A480-6D47-8865-EF09DF86D2D2}"/>
     <hyperlink ref="E56" r:id="rId2" xr:uid="{D1356C83-4F55-6C4F-825F-182E36883A34}"/>
-    <hyperlink ref="E35" r:id="rId3" display="https://www.atlas-lithium.com/news/atlas-lithium-intersects-wide-high-grade-lithium-mineralization-continues-expansion-of-anitta-3-and-anitta-4-pegmatites/" xr:uid="{8852D753-D43D-5343-9964-585CBF8A8AA0}"/>
+    <hyperlink ref="E36" r:id="rId3" display="https://www.atlas-lithium.com/news/atlas-lithium-intersects-wide-high-grade-lithium-mineralization-continues-expansion-of-anitta-3-and-anitta-4-pegmatites/" xr:uid="{8852D753-D43D-5343-9964-585CBF8A8AA0}"/>
+    <hyperlink ref="E35" r:id="rId4" display="https://www.atlas-lithium.com/news/atlas-lithiums-modular-processing-plant-enters-final-fabrication-and-trial-assembly-stage/" xr:uid="{1F8029A1-EABA-624B-8164-CA81B9E772AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -791,19 +802,19 @@
   <sheetData>
     <row r="3" spans="2:6">
       <c r="B3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:6">

</xml_diff>